<commit_message>
更新配置档字符编码为utf-8 without bom; buglist.xlsx 新增QA
</commit_message>
<xml_diff>
--- a/VGALightStripDetection/testbat/buglist.xlsx
+++ b/VGALightStripDetection/testbat/buglist.xlsx
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Item</t>
   </si>
@@ -350,6 +350,27 @@
   <si>
     <t>获取background 耗时105ms; 获取foreground 耗时164ms;从图片中能看到background 中残留着上一轮未灭完的蓝灯</t>
   </si>
+  <si>
+    <t>2.0.1.8</t>
+  </si>
+  <si>
+    <t>测试TUF-RX6800XT 100% 1006
+debug 显示 call PADL_Display_WriteAndReadI2C return -5
+/// Invalid ADL index passed
+#define ADL_ERR_INVALID_ADL_IDX            -5
+将问题卡插入开发平台后报1006; 
+将之前开发用的TUF-RX6800 插入开发平台后也突然报1006;将借到的两张TUF-RX6800XT 插入开发平台也报1006;
+用历史版本对开发用的TUF-RX6800 进行复测, 报1006(之前是OK的);
+将开发用的TUF-RX6800 插入Jake 测试平台, 安装驱动后, 测试pass;
+将开发用的TUF-RX6800 插入开发平台, 安装最新驱动, 同时卸载A卡旧版本驱动, 测试pass</t>
+  </si>
+  <si>
+    <t>从复验过程上看, 应该是驱动出问题了;
+对于出问题的TUF-RX6800XT测试1006; 再验开发用的TUF-6800测试1006; 这一现象来看, 推测应该是TUF-RX6800XT 引起驱动识别混乱, 造成后续全部集中都测不过</t>
+  </si>
+  <si>
+    <t>在测试系统盘上, 重新安装A卡驱动, 同时设置删除历史驱动</t>
+  </si>
 </sst>
 </file>
 
@@ -357,8 +378,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -382,6 +403,42 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -407,7 +464,76 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -418,111 +544,6 @@
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -548,187 +569,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,39 +760,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -790,21 +778,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -812,6 +785,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -839,6 +821,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -847,10 +868,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -859,137 +880,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1015,13 +1036,10 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1371,12 +1389,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1643,7 +1661,7 @@
       <c r="D20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="6" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1654,13 +1672,13 @@
       <c r="C21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="6" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1671,13 +1689,30 @@
       <c r="C22" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="10"/>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" ht="256.5" spans="2:7">
+      <c r="B23" s="5">
+        <v>44540</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>